<commit_message>
Working reading from excel and searching for their folders
</commit_message>
<xml_diff>
--- a/subslist.xlsx
+++ b/subslist.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t xml:space="preserve">ID Number</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t xml:space="preserve">ID NUMBER</t>
   </si>
   <si>
     <t xml:space="preserve">Last Name</t>
@@ -35,6 +35,39 @@
   </si>
   <si>
     <t xml:space="preserve">Google Drive Shareable link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORPILLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBRIEL RENZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CABALLEROS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PALER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NATHALIE KATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZIRELLE DOMINIQUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAPUZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZAMANTHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOLENDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEO</t>
   </si>
 </sst>
 </file>
@@ -44,7 +77,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -64,6 +97,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,9 +146,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -130,10 +172,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="310" zoomScaleNormal="310" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -158,6 +200,64 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>20190016812</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>20170012416</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>20170011560</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>20170011644</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>20150007960</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>